<commit_message>
[2020-10-21 10:48] Read & Write Using Openpyxl
</commit_message>
<xml_diff>
--- a/export/test.xlsx
+++ b/export/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10yeo\Documents\Github\python-practice\export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kyh\py_workspace\python-practice\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342BDCAC-27BA-4DF2-84AA-D90308CB71F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78990032-D354-4007-93BB-B0A4AFCD379E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,30 +23,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>바</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>이름</t>
+  </si>
+  <si>
+    <t>사는 곳</t>
+  </si>
+  <si>
+    <t>직업</t>
+  </si>
+  <si>
+    <t>Elsa</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>Lawyer</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Programmer</t>
+  </si>
+  <si>
+    <t>Olaf</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Busan</t>
+  </si>
+  <si>
+    <t>Designer</t>
   </si>
 </sst>
 </file>
@@ -396,32 +426,95 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.75" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>